<commit_message>
BCHoaHong DVDacBiet: thêm 1 số cột + check vượt mức
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Report/BaoCaoChietKhau/Temp_BaoCaoHoaHongDoanhThu.xlsx
+++ b/banhang24/Template/ExportExcel/Report/BaoCaoChietKhau/Temp_BaoCaoHoaHongDoanhThu.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Mã nhân viên</t>
   </si>
@@ -32,13 +32,16 @@
     <t>Tên nhân viên</t>
   </si>
   <si>
-    <t>Hoa hồng doanh thu</t>
-  </si>
-  <si>
     <t>Tổng cộng</t>
   </si>
   <si>
     <t>BÁO CÁO HOA HỒNG NHÂN VIÊN THEO DOANH THU</t>
+  </si>
+  <si>
+    <t>Hoa hồng</t>
+  </si>
+  <si>
+    <t>Doanh số hưởng</t>
   </si>
 </sst>
 </file>
@@ -141,7 +144,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -189,6 +192,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -471,37 +483,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C2"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.28515625" style="13" customWidth="1"/>
     <col min="2" max="2" width="41.28515625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" style="15" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="2"/>
+    <col min="3" max="3" width="28.42578125" style="18" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" style="15" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D1" s="17"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="17"/>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D2" s="17"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
     </row>
-    <row r="4" spans="1:4" s="14" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="14" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
@@ -509,144 +524,173 @@
         <v>1</v>
       </c>
       <c r="C4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="10"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="10"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="10"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="10"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="10"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="10"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="10"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="10"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="10"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="10"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="10"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="10"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="10"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="10"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="10"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="10"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="10"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="10"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="10"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="10"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="10"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="8"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="10"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="8"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="10"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="8"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="10"/>
+    </row>
+    <row r="29" spans="1:4" s="12" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="16" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="10"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="10"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="10"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="10"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="10"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="10"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="10"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="10"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="10"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="10"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="10"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="10"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="10"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="10"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="10"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="10"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="10"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="10"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="10"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="10"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="10"/>
-    </row>
-    <row r="29" spans="1:3" s="12" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="16" t="s">
-        <v>3</v>
-      </c>
       <c r="B29" s="16"/>
-      <c r="C29" s="11">
-        <f>SUM(C$5:C28)</f>
+      <c r="C29" s="20"/>
+      <c r="D29" s="11">
+        <f>SUM(D$5:D28)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="A1:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>